<commit_message>
Testing commit as Lee
</commit_message>
<xml_diff>
--- a/CardiologyData.xlsx
+++ b/CardiologyData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RCA1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\YEAR 4\Semester 8\Enterprise Dataset Technologies\RCA1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -117,8 +117,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -146,8 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +439,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -438,51 +449,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
@@ -529,56 +540,57 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
min, max, mean, median, sd done
</commit_message>
<xml_diff>
--- a/CardiologyData.xlsx
+++ b/CardiologyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>age</t>
   </si>
@@ -196,9 +196,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,9 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -592,6 +591,51 @@
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>6.4000000000000003E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -744,6 +788,51 @@
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B7">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>120</v>
+      </c>
+      <c r="F7">
+        <v>204</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7">
+        <v>76.8</v>
+      </c>
+      <c r="J7">
+        <v>162</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -798,6 +887,51 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="B9">
+        <v>9.7759420000000006</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <v>17.490020000000001</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9">
+        <v>0.35378510000000002</v>
+      </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9">
+        <v>10.718159999999999</v>
+      </c>
+      <c r="J9">
+        <v>22.768049999999999</v>
+      </c>
+      <c r="K9">
+        <v>0.46901540000000003</v>
+      </c>
+      <c r="L9">
+        <v>1.166037</v>
+      </c>
+      <c r="M9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9">
+        <v>0.93121889999999996</v>
+      </c>
+      <c r="O9" t="s">
+        <v>36</v>
+      </c>
+      <c r="P9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
q1 and 2 finished
</commit_message>
<xml_diff>
--- a/CardiologyData.xlsx
+++ b/CardiologyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
   <si>
     <t>age</t>
   </si>
@@ -110,9 +110,6 @@
     <t xml:space="preserve">Is numeric data skewed? Type </t>
   </si>
   <si>
-    <t xml:space="preserve">Level of correlation </t>
-  </si>
-  <si>
     <t>NoTang</t>
   </si>
   <si>
@@ -153,6 +150,42 @@
   </si>
   <si>
     <t>Healthy</t>
+  </si>
+  <si>
+    <t>Positively Skewed</t>
+  </si>
+  <si>
+    <t>Negatively Skewed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometric </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes, Positively</t>
+  </si>
+  <si>
+    <t>Yes, Negatively</t>
+  </si>
+  <si>
+    <t>0.2385335 diastbpexerc</t>
+  </si>
+  <si>
+    <t>Level of correlation (Highest)</t>
+  </si>
+  <si>
+    <t>0.9505095 diastbpexerc</t>
+  </si>
+  <si>
+    <t>0.9505095 trestbps</t>
+  </si>
+  <si>
+    <t>-0.04608416 trestbps</t>
+  </si>
+  <si>
+    <t>0.2164572 age</t>
   </si>
 </sst>
 </file>
@@ -196,10 +229,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,11 +516,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -534,7 +576,7 @@
         <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -645,10 +687,10 @@
         <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>200</v>
@@ -660,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4">
         <v>128</v>
@@ -675,16 +717,16 @@
         <v>6.2</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4">
         <v>3</v>
       </c>
       <c r="O4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" t="s">
         <v>33</v>
-      </c>
-      <c r="P4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -695,10 +737,10 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
       </c>
       <c r="E5">
         <v>94</v>
@@ -710,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5">
         <v>60.16</v>
@@ -725,16 +767,16 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
         <v>40</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>41</v>
-      </c>
-      <c r="P5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -745,10 +787,10 @@
         <v>54.237009999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6">
         <v>131.43180000000001</v>
@@ -772,16 +814,16 @@
         <v>1.0493509999999999</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N6">
         <v>0.66883119999999996</v>
       </c>
       <c r="O6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -792,10 +834,10 @@
         <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>120</v>
@@ -807,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7">
         <v>76.8</v>
@@ -822,16 +864,16 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -842,10 +884,10 @@
         <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>130</v>
@@ -857,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8">
         <v>83.2</v>
@@ -872,16 +914,16 @@
         <v>0.8</v>
       </c>
       <c r="M8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -892,22 +934,22 @@
         <v>9.7759420000000006</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9">
         <v>17.490020000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9">
         <v>0.35378510000000002</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9">
         <v>10.718159999999999</v>
@@ -922,31 +964,166 @@
         <v>1.166037</v>
       </c>
       <c r="M9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N9">
         <v>0.93121889999999996</v>
       </c>
       <c r="O9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
q1 - 5 done, actually little bit of 4 to do
</commit_message>
<xml_diff>
--- a/CardiologyData.xlsx
+++ b/CardiologyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
   <si>
     <t>age</t>
   </si>
@@ -152,15 +152,6 @@
     <t>Healthy</t>
   </si>
   <si>
-    <t>Positively Skewed</t>
-  </si>
-  <si>
-    <t>Negatively Skewed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometric </t>
-  </si>
-  <si>
     <t>0.2385335 diastbpexerc</t>
   </si>
   <si>
@@ -195,6 +186,33 @@
   </si>
   <si>
     <t>1.229654, Positively</t>
+  </si>
+  <si>
+    <t>p-value = 0.0007914 -&gt; Deviates From Normality</t>
+  </si>
+  <si>
+    <t>p-value = 8.431e-07 -&gt; Normal Distribution</t>
+  </si>
+  <si>
+    <t>p-value = 4.548e-09 -&gt; Normal Distribution</t>
+  </si>
+  <si>
+    <t>p-value = 3.104e-07 -&gt; Normal Distribution</t>
+  </si>
+  <si>
+    <t>p-value = 5.608e-05 -&gt; Normal Distribution</t>
+  </si>
+  <si>
+    <t>p-value &lt; 2.2e-16 -&gt; Deviates From Normal Distribution</t>
+  </si>
+  <si>
+    <t>p-value &lt; 2.2e-16 -&gt; Deviates From Normality</t>
+  </si>
+  <si>
+    <t>1.186547, Positively</t>
+  </si>
+  <si>
+    <t>0.3120721 age</t>
   </si>
 </sst>
 </file>
@@ -526,18 +544,23 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -990,7 +1013,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
@@ -999,10 +1022,10 @@
         <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
         <v>35</v>
@@ -1011,22 +1034,22 @@
         <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
         <v>35</v>
       </c>
       <c r="L10" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="M10" t="s">
         <v>35</v>
       </c>
       <c r="N10" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="O10" t="s">
         <v>35</v>
@@ -1040,43 +1063,43 @@
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="J11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F11" t="s">
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" t="s">
         <v>53</v>
       </c>
-      <c r="G11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" t="s">
-        <v>56</v>
-      </c>
       <c r="M11" t="s">
         <v>35</v>
       </c>
       <c r="N11" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="O11" t="s">
         <v>35</v>
@@ -1087,46 +1110,46 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" t="s">
         <v>47</v>
       </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" t="s">
-        <v>50</v>
-      </c>
       <c r="M12" t="s">
         <v>35</v>
       </c>
       <c r="N12" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="O12" t="s">
         <v>35</v>

</xml_diff>